<commit_message>
update 20230517 by xhx
</commit_message>
<xml_diff>
--- a/rules/rules_pID-1.xlsx
+++ b/rules/rules_pID-1.xlsx
@@ -215,7 +215,7 @@
         <v>1080</v>
       </c>
       <c r="K3" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -248,7 +248,7 @@
         <v>1080</v>
       </c>
       <c r="K4" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -281,7 +281,7 @@
         <v>1080</v>
       </c>
       <c r="K5" s="0">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -314,7 +314,7 @@
         <v>1080</v>
       </c>
       <c r="K6" s="0">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -380,7 +380,7 @@
         <v>12000</v>
       </c>
       <c r="K8" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -413,7 +413,7 @@
         <v>12000</v>
       </c>
       <c r="K9" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -446,7 +446,7 @@
         <v>12000</v>
       </c>
       <c r="K10" s="0">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -479,7 +479,7 @@
         <v>12000</v>
       </c>
       <c r="K11" s="0">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -545,7 +545,7 @@
         <v>22920</v>
       </c>
       <c r="K13" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -578,7 +578,7 @@
         <v>22920</v>
       </c>
       <c r="K14" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
@@ -611,7 +611,7 @@
         <v>22920</v>
       </c>
       <c r="K15" s="0">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -644,7 +644,7 @@
         <v>22920</v>
       </c>
       <c r="K16" s="0">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">

</xml_diff>